<commit_message>
Add Expression Zone logic
</commit_message>
<xml_diff>
--- a/Assets/Data/fieldRule.xlsx
+++ b/Assets/Data/fieldRule.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="7800"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="7800" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="4" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
 </workbook>
@@ -79,8 +80,46 @@
 </comments>
 </file>
 
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>吴冠杰.Mike</author>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>吴冠杰.Mike:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t xml:space="preserve">
+1目标类型
+2表达式
+100 通用条件</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="72">
   <si>
     <t>字段英文名</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -195,6 +234,178 @@
   </si>
   <si>
     <t>周期生效时效果2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>caster</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>自身</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>add_hurt</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>add_hurt_when_a</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>造成伤害</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>无条件</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>枚举显示文本</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>枚举字段</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>枚举类别</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>无目标</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>friend</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>友方</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>target</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>敌方</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>global</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>第一对象</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>造成伤害单条件</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>参数个数</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>参数说明</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>伤害id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>条件类型#条件参数#伤害id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>参数涉及枚举类型</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>100#0#0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>施法者不拥有某个BUFF(buff_id)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>施法者拥有某个BUFF(buff_id)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>生效目标拥有某个BUFF(buff_id)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>生效目标不拥有某个BUFF(buff_id)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>生效目标是玩家</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>生效目标是怪物</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>add_hurt_when_a_and_b</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>造成伤害双条件</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>mowing</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>割草</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>条件类型1#条件参数1#条件类型2#条件参数2#伤害id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>100#0#100#0#0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>add_buff</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>add_buff_when_a</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>添加Buff</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>添加Buff单条件</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>概率#buffid#buff时长</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>条件类型1#条件参数1概率#buffid#buff时长</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>100#0#0#0#0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0#0#0</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -202,7 +413,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -228,6 +439,21 @@
       <sz val="9"/>
       <color indexed="81"/>
       <name val="宋体"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="宋体"/>
+      <family val="3"/>
       <charset val="134"/>
     </font>
   </fonts>
@@ -542,8 +768,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -759,4 +985,294 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="9" style="1"/>
+    <col min="2" max="2" width="27" style="1" customWidth="1"/>
+    <col min="3" max="3" width="34.25" style="1" customWidth="1"/>
+    <col min="4" max="4" width="17.875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="51" style="1" customWidth="1"/>
+    <col min="6" max="6" width="22.875" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="9" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
+        <v>1</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
+        <v>1</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
+        <v>1</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" s="1">
+        <v>2</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7" s="1">
+        <v>1</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F7" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" s="1">
+        <v>2</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D8" s="1">
+        <v>3</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" s="1">
+        <v>2</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D9" s="1">
+        <v>5</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" s="1">
+        <v>2</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D10" s="1">
+        <v>3</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" s="1">
+        <v>2</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D11" s="1">
+        <v>5</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" s="1">
+        <v>2</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D12" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" s="1">
+        <v>100</v>
+      </c>
+      <c r="B13" s="1">
+        <v>0</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" s="1">
+        <v>100</v>
+      </c>
+      <c r="B14" s="1">
+        <v>1</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" s="1">
+        <v>100</v>
+      </c>
+      <c r="B15" s="1">
+        <v>2</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" s="1">
+        <v>100</v>
+      </c>
+      <c r="B16" s="1">
+        <v>3</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" s="1">
+        <v>100</v>
+      </c>
+      <c r="B17" s="1">
+        <v>4</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" s="1">
+        <v>100</v>
+      </c>
+      <c r="B18" s="1">
+        <v>5</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" s="1">
+        <v>100</v>
+      </c>
+      <c r="B19" s="1">
+        <v>6</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>